<commit_message>
Inclui 'Retificação' no dicionário de tipos de normas
</commit_message>
<xml_diff>
--- a/R/rDOU/inst/extdata/des_tipo.xlsx
+++ b/R/rDOU/inst/extdata/des_tipo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa.goncalves\Desktop\Doc_SISLEGIS\Exportações\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas.barcellos\Desktop\Projetos\Controle\projdiario\R\rDOU\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="955">
   <si>
     <t>SGL_TIPO</t>
   </si>
@@ -2884,12 +2884,15 @@
   </si>
   <si>
     <t>Diretriz Ministerial</t>
+  </si>
+  <si>
+    <t>Retificação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2919,8 +2922,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3204,10 +3208,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B491"/>
+  <dimension ref="A1:B492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183"/>
+    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
+      <selection activeCell="A492" sqref="A492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7143,6 +7147,14 @@
         <v>482</v>
       </c>
     </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B492" t="s">
+        <v>954</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1">
     <sortState ref="A2:B491">

</xml_diff>